<commit_message>
lowest point and reason analysis
</commit_message>
<xml_diff>
--- a/actual_data/domestic.xlsx
+++ b/actual_data/domestic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d9d98fa56c37d9d/ドキュメント/GitHub/lab/actual_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univtokyo-my.sharepoint.com/personal/1003519251_utac_u-tokyo_ac_jp/Documents/ドキュメント/GitHub/lab/actual_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_AD4D066CA252ABDACC10485A2151EF8673EEDF5F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA70BCD3-7EEB-4D83-83B9-01743C759873}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_AD4D066CA252ABDACC10485A2151EF8673EEDF5F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1C50B4C-B415-4D0A-AB39-8ED51783994E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="22040" yWindow="-610" windowWidth="23260" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="可視化" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2051,10 +2051,13 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="22.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">

</xml_diff>